<commit_message>
Changed ms to sec
</commit_message>
<xml_diff>
--- a/Data/PerformData.xlsx
+++ b/Data/PerformData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,6 @@
     <t>load</t>
   </si>
   <si>
-    <t>test student</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
     <t>step 1</t>
   </si>
   <si>
@@ -71,7 +65,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>IE</t>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,50 +467,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -518,9 +521,7 @@
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="E2" s="6"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
       <c r="H2" s="5"/>

</xml_diff>